<commit_message>
added template and system architecture
</commit_message>
<xml_diff>
--- a/trunk/Documentation/ProjectDocumentation/Website_template.xlsx
+++ b/trunk/Documentation/ProjectDocumentation/Website_template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Desktop\aerojump\aerojump\trunk\Documentation\ProjectDocumentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="15" windowWidth="19320" windowHeight="14520"/>
   </bookViews>
@@ -78,9 +83,6 @@
     <t>Freigabe</t>
   </si>
   <si>
-    <t>Martina Musterfrau, Max Mustermann</t>
-  </si>
-  <si>
     <t>FH-Studenten</t>
   </si>
   <si>
@@ -96,24 +98,12 @@
     <t>Vollständiger Titel und Name des Projektbetreuers</t>
   </si>
   <si>
-    <t>Musterfirma</t>
-  </si>
-  <si>
     <t>Hier soll eine Kurzbeschreibung des Projekts eingefügt werden. Dieser Kurztext wird neben dem Logo des Projekts (1. Bild) auf der Projektübersichtsseite zu lesen sein. Die Länge sollte ca. 2-3 Sätze betragen.</t>
   </si>
   <si>
-    <t>Mustertitel</t>
-  </si>
-  <si>
-    <t>DI Dr. Max Mustermann, BSc, MSc</t>
-  </si>
-  <si>
     <t>Liste der Namen der Studierenden, die an diesem Projekt mitarbeiten, mit Komma getrennt.</t>
   </si>
   <si>
-    <t>Bild1.jpg,Bild2.png,Bild3.gif</t>
-  </si>
-  <si>
     <t>Ausfüllhinweise: Für 1 Projekt muss jeweils 1 Zeile ausgefüllt werden. Zu verwenden ist die obige Zeile mit den Musterdaten. Die ausgeblendeten Spalten sollen nicht eingeblendet werden.</t>
   </si>
   <si>
@@ -132,24 +122,38 @@
     <t>Bei Unklarheiten können die aktuellen Projektbeschreibungen auf der Website als Referenz herangezogen werden. Bei konkreten Fragen ist Kontakt mit Stephan Drab aufzunehmen.</t>
   </si>
   <si>
-    <t>Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext.
-Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext.</t>
-  </si>
-  <si>
-    <t>Dies ist eine Musterkurzbeschreibung. Dies ist eine Musterkurzbeschreibung.</t>
-  </si>
-  <si>
-    <t>Sommersemester 2009</t>
-  </si>
-  <si>
     <t>abgeschlossen</t>
+  </si>
+  <si>
+    <t>AeroJump</t>
+  </si>
+  <si>
+    <t>Sommersemester 2017</t>
+  </si>
+  <si>
+    <t>AeroJump ist ein Jump'n'Run Game für Android.</t>
+  </si>
+  <si>
+    <t>Marko Bliznac, Peter Elsigan, David Mitterlehner</t>
+  </si>
+  <si>
+    <t>Markus Altenhuber</t>
+  </si>
+  <si>
+    <t>Keine</t>
+  </si>
+  <si>
+    <t>Das Ziel des Projektes ist die Umsetzung eines Jump 'n' Run Spiels für Android.</t>
+  </si>
+  <si>
+    <t>Homepage ist keine vorhanden.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -298,15 +302,89 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1057275</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3024B493-138B-4530-A94C-AF933F263B8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1628775" y="190500"/>
+          <a:ext cx="485775" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -348,7 +426,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -380,9 +458,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -414,6 +510,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -589,14 +703,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
@@ -620,7 +734,7 @@
     <col min="20" max="20" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1">
+    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -682,50 +796,50 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="6" customFormat="1" ht="12.75" customHeight="1">
+    <row r="2" spans="1:20" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H2" s="6">
         <v>0</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="T2" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="6" customFormat="1"/>
-    <row r="4" spans="1:20" s="6" customFormat="1"/>
-    <row r="5" spans="1:20" s="6" customFormat="1"/>
-    <row r="6" spans="1:20">
+    <row r="3" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -742,12 +856,12 @@
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -763,12 +877,12 @@
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
     </row>
-    <row r="8" spans="1:20" ht="52.5" customHeight="1">
+    <row r="8" spans="1:20" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -784,12 +898,12 @@
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
     </row>
-    <row r="9" spans="1:20" ht="27.75" customHeight="1">
+    <row r="9" spans="1:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -805,12 +919,12 @@
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -826,12 +940,12 @@
       <c r="N10" s="13"/>
       <c r="O10" s="14"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -847,12 +961,12 @@
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -868,12 +982,12 @@
       <c r="N12" s="11"/>
       <c r="O12" s="11"/>
     </row>
-    <row r="13" spans="1:20" ht="39" customHeight="1">
+    <row r="13" spans="1:20" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -889,9 +1003,9 @@
       <c r="N13" s="15"/>
       <c r="O13" s="15"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -925,16 +1039,17 @@
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
@@ -943,12 +1058,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>

</xml_diff>